<commit_message>
added Median_hillow function to my plot
</commit_message>
<xml_diff>
--- a/Data/maps.xlsx
+++ b/Data/maps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="Farms" sheetId="4" r:id="rId1"/>
@@ -21,25 +21,239 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="66">
   <si>
     <t>S/N</t>
   </si>
   <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>LGA</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
     <t>Elevation (m)</t>
   </si>
   <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Latitude</t>
+    <t>Oyo</t>
+  </si>
+  <si>
+    <t>Akinyele</t>
+  </si>
+  <si>
+    <t>Oluyole</t>
+  </si>
+  <si>
+    <t>Ogbomoso North</t>
+  </si>
+  <si>
+    <t>Ogbomoso South</t>
+  </si>
+  <si>
+    <t>Ekiti</t>
+  </si>
+  <si>
+    <t>Ekiti East</t>
+  </si>
+  <si>
+    <t>Gbonyin</t>
+  </si>
+  <si>
+    <t>Ondo</t>
+  </si>
+  <si>
+    <t>Akure North</t>
+  </si>
+  <si>
+    <t>Owo</t>
+  </si>
+  <si>
+    <t>Kwara</t>
+  </si>
+  <si>
+    <t>Ilorin South</t>
+  </si>
+  <si>
+    <t>Akwa Ibom</t>
+  </si>
+  <si>
+    <t>Itu</t>
+  </si>
+  <si>
+    <t>Uyo</t>
+  </si>
+  <si>
+    <t>Ibiono Ibom</t>
+  </si>
+  <si>
+    <t>Ebonyi</t>
+  </si>
+  <si>
+    <t>Ohaukwu</t>
+  </si>
+  <si>
+    <t>Ezza North</t>
+  </si>
+  <si>
+    <t>Abakaliki</t>
+  </si>
+  <si>
+    <t>Anambra</t>
+  </si>
+  <si>
+    <t>Idemili South</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Bodija</t>
+  </si>
+  <si>
+    <t>Okesa</t>
+  </si>
+  <si>
+    <t>Oja Oba</t>
+  </si>
+  <si>
+    <t>Kota-Omuo</t>
+  </si>
+  <si>
+    <t>Ogbese</t>
+  </si>
+  <si>
+    <t>Plaza</t>
+  </si>
+  <si>
+    <t>Iboko</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Eke</t>
+  </si>
+  <si>
+    <t>Community_Market</t>
+  </si>
+  <si>
+    <t>Idi Ose</t>
+  </si>
+  <si>
+    <t>Sagbe</t>
+  </si>
+  <si>
+    <t>Idi Ayunre</t>
+  </si>
+  <si>
+    <t>Sabo</t>
+  </si>
+  <si>
+    <t>Sun-unsun-un</t>
+  </si>
+  <si>
+    <t>Eda-Ile</t>
+  </si>
+  <si>
+    <t>Ilu Omooba</t>
+  </si>
+  <si>
+    <t>Bolunrunduro</t>
+  </si>
+  <si>
+    <t>Amure</t>
+  </si>
+  <si>
+    <t>Oke Yalu</t>
+  </si>
+  <si>
+    <t>Asa</t>
+  </si>
+  <si>
+    <t>Nwtusiong</t>
+  </si>
+  <si>
+    <t>Ikot Ekpuk</t>
+  </si>
+  <si>
+    <t>Itam</t>
+  </si>
+  <si>
+    <t>Nung obio enang</t>
+  </si>
+  <si>
+    <t>Ikot Idaha</t>
+  </si>
+  <si>
+    <t>Ntuskpa</t>
+  </si>
+  <si>
+    <t>Nwankuu Ntsurakpa Izhia</t>
+  </si>
+  <si>
+    <t>Umueghara</t>
+  </si>
+  <si>
+    <t>Ezzangwu Amaechi</t>
+  </si>
+  <si>
+    <t>Oshiegbe</t>
+  </si>
+  <si>
+    <t>Umu ezeohohoa</t>
+  </si>
+  <si>
+    <t>Agbaja Azumili</t>
+  </si>
+  <si>
+    <r>
+      <t>Unagboke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Egugwu Agbaja</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>unhufu</t>
+    </r>
+  </si>
+  <si>
+    <t>Uke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,7 +265,38 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -59,17 +304,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,12 +317,120 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79992065187536243"/>
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6DCE4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B084"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACB9CA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79989013336588644"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -119,43 +466,141 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,771 +877,1095 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="10.5703125"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125"/>
+    <col min="6" max="6" width="12.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" s="41" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="45">
         <v>7.5082592999999997</v>
       </c>
-      <c r="C2" s="4">
+      <c r="E2" s="45">
         <v>3.9131901999999998</v>
       </c>
-      <c r="D2" s="4">
+      <c r="F2" s="45">
         <v>262.11297999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="45">
         <v>7.4930361999999997</v>
       </c>
-      <c r="C3" s="4">
+      <c r="E3" s="45">
         <v>3.9171141</v>
       </c>
-      <c r="D3" s="4">
+      <c r="F3" s="45">
         <v>222.8452494</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="45">
         <v>7.4973277999999999</v>
       </c>
-      <c r="C4" s="4">
+      <c r="E4" s="45">
         <v>3.9137483</v>
       </c>
-      <c r="D4" s="4">
+      <c r="F4" s="45">
         <v>254.18005959999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="45">
         <v>7.2126675999999996</v>
       </c>
-      <c r="C5" s="4">
+      <c r="E5" s="45">
         <v>3.8560881999999999</v>
       </c>
-      <c r="D5" s="4">
+      <c r="F5" s="45">
         <v>137.0534126</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="45">
         <v>8.1469462999999998</v>
       </c>
-      <c r="C6" s="4">
+      <c r="E6" s="45">
         <v>4.2385128999999999</v>
       </c>
-      <c r="D6" s="4">
+      <c r="F6" s="45">
         <v>350.97296460000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="45">
         <v>8.1492085999999997</v>
       </c>
-      <c r="C7" s="4">
+      <c r="E7" s="45">
         <v>4.2394099000000001</v>
       </c>
-      <c r="D7" s="4">
+      <c r="F7" s="45">
         <v>348.40469519999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="45">
         <v>8.1447479999999999</v>
       </c>
-      <c r="C8" s="4">
+      <c r="E8" s="45">
         <v>4.2379898000000003</v>
       </c>
-      <c r="D8" s="4">
+      <c r="F8" s="45">
         <v>351.41592589999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="45">
         <v>8.1054720000000007</v>
       </c>
-      <c r="C9" s="4">
+      <c r="E9" s="45">
         <v>4.2349439999999996</v>
       </c>
-      <c r="D9" s="4">
+      <c r="F9" s="45">
         <v>346.33139999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="45">
         <v>7.7577058000000001</v>
       </c>
-      <c r="C10" s="4">
+      <c r="E10" s="45">
         <v>5.7216997999999997</v>
       </c>
-      <c r="D10" s="4">
+      <c r="F10" s="45">
         <v>562.48781320000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="45">
         <v>7.7487288999999997</v>
       </c>
-      <c r="C11" s="4">
+      <c r="E11" s="45">
         <v>5.6428988999999996</v>
       </c>
-      <c r="D11" s="4">
+      <c r="F11" s="45">
         <v>565.17999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="45">
         <v>7.7410205000000003</v>
       </c>
-      <c r="C12" s="4">
+      <c r="E12" s="45">
         <v>5.6431851999999996</v>
       </c>
-      <c r="D12" s="4">
+      <c r="F12" s="45">
         <v>552.81183450000003</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="45">
         <v>7.7408146000000002</v>
       </c>
-      <c r="C13" s="4">
+      <c r="E13" s="45">
         <v>5.6435231999999997</v>
       </c>
-      <c r="D13" s="4">
+      <c r="F13" s="45">
         <v>553.31475450000005</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="45">
         <v>7.6322823</v>
       </c>
-      <c r="C14" s="4">
+      <c r="E14" s="45">
         <v>5.4214238999999997</v>
       </c>
-      <c r="D14" s="4">
+      <c r="F14" s="45">
         <v>419.95606720000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="45">
         <v>7.6383270999999997</v>
       </c>
-      <c r="C15" s="4">
+      <c r="E15" s="45">
         <v>5.4228630999999998</v>
       </c>
-      <c r="D15" s="4">
+      <c r="F15" s="45">
         <v>414.038365</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="45">
         <v>7.2208299</v>
       </c>
-      <c r="C16" s="4">
+      <c r="E16" s="45">
         <v>5.4022946000000003</v>
       </c>
-      <c r="D16" s="4">
+      <c r="F16" s="45">
         <v>335.24253620000002</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="45">
         <v>7.2155867999999996</v>
       </c>
-      <c r="C17" s="4">
+      <c r="E17" s="45">
         <v>5.4057706000000003</v>
       </c>
-      <c r="D17" s="4">
+      <c r="F17" s="45">
         <v>335.26</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="45">
         <v>7.2598403999999999</v>
       </c>
-      <c r="C18" s="4">
+      <c r="E18" s="45">
         <v>5.4763064999999997</v>
       </c>
-      <c r="D18" s="4">
+      <c r="F18" s="45">
         <v>323.38337999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="45">
         <v>8.4588055000000004</v>
       </c>
-      <c r="C19" s="4">
+      <c r="E19" s="45">
         <v>4.5871690000000003</v>
       </c>
-      <c r="D19" s="4">
+      <c r="F19" s="45">
         <v>337.45238499999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="45">
         <v>8.4586360999999997</v>
       </c>
-      <c r="C20" s="4">
+      <c r="E20" s="45">
         <v>4.5855233000000002</v>
       </c>
-      <c r="D20" s="4">
+      <c r="F20" s="45">
         <v>332.19378169999999</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="45">
         <v>8.4582362999999994</v>
       </c>
-      <c r="C21" s="4">
+      <c r="E21" s="45">
         <v>4.5883664</v>
       </c>
-      <c r="D21" s="4">
+      <c r="F21" s="45">
         <v>333.20462409999999</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="45">
         <v>8.4580994</v>
       </c>
-      <c r="C22" s="4">
+      <c r="E22" s="45">
         <v>4.5897059000000002</v>
       </c>
-      <c r="D22" s="4">
+      <c r="F22" s="45">
         <v>306.33999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="45">
         <v>5.0544343999999999</v>
       </c>
-      <c r="C23" s="4">
+      <c r="E23" s="45">
         <v>7.9043095000000001</v>
       </c>
-      <c r="D23" s="4">
+      <c r="F23" s="45">
         <v>78.057799200000005</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="45">
         <v>5.0571232000000004</v>
       </c>
-      <c r="C24" s="4">
+      <c r="E24" s="45">
         <v>7.9037034999999998</v>
       </c>
-      <c r="D24" s="4">
+      <c r="F24" s="45">
         <v>92.203197009999997</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="45">
         <v>5.0560362999999997</v>
       </c>
-      <c r="C25" s="4">
+      <c r="E25" s="45">
         <v>7.9007921999999997</v>
       </c>
-      <c r="D25" s="4">
+      <c r="F25" s="45">
         <v>87.837404199999995</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="45">
         <v>5.0577817999999999</v>
       </c>
-      <c r="C26" s="4">
+      <c r="E26" s="45">
         <v>7.9020660999999999</v>
       </c>
-      <c r="D26" s="4">
+      <c r="F26" s="45">
         <v>90.913150470000005</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="45">
         <v>5.0546939000000002</v>
       </c>
-      <c r="C27" s="4">
+      <c r="E27" s="45">
         <v>7.9160988000000003</v>
       </c>
-      <c r="D27" s="4">
+      <c r="F27" s="45">
         <v>93.96233909</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="45">
         <v>5.0434536000000003</v>
       </c>
-      <c r="C28" s="4">
+      <c r="E28" s="45">
         <v>7.8791330000000004</v>
       </c>
-      <c r="D28" s="4">
+      <c r="F28" s="45">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="45">
         <v>5.0400241000000001</v>
       </c>
-      <c r="C29" s="4">
+      <c r="E29" s="45">
         <v>7.8734451999999999</v>
       </c>
-      <c r="D29" s="4">
+      <c r="F29" s="45">
         <v>81.819504260000002</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="45">
         <v>5.0406405999999997</v>
       </c>
-      <c r="C30" s="4">
+      <c r="E30" s="45">
         <v>7.8738900000000003</v>
       </c>
-      <c r="D30" s="4">
+      <c r="F30" s="45">
         <v>85.720904570000002</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="45">
         <v>5.0409587</v>
       </c>
-      <c r="C31" s="4">
+      <c r="E31" s="45">
         <v>7.8737336999999998</v>
       </c>
-      <c r="D31" s="4">
+      <c r="F31" s="45">
         <v>84.218533309999998</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="45">
         <v>5.0410715000000001</v>
       </c>
-      <c r="C32" s="4">
+      <c r="E32" s="45">
         <v>7.8727042999999997</v>
       </c>
-      <c r="D32" s="4">
+      <c r="F32" s="45">
         <v>82.90707639</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="45">
         <v>5.0411717999999999</v>
       </c>
-      <c r="C33" s="4">
+      <c r="E33" s="45">
         <v>7.8724673000000003</v>
       </c>
-      <c r="D33" s="4">
+      <c r="F33" s="45">
         <v>79.798794009999995</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="45">
         <v>5.0422811000000003</v>
       </c>
-      <c r="C34" s="4">
+      <c r="E34" s="45">
         <v>7.8696457000000004</v>
       </c>
-      <c r="D34" s="4">
+      <c r="F34" s="45">
         <v>72.167455590000003</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="45">
         <v>5.0422913999999999</v>
       </c>
-      <c r="C35" s="4">
+      <c r="E35" s="45">
         <v>7.8696792000000002</v>
       </c>
-      <c r="D35" s="4">
+      <c r="F35" s="45">
         <v>78.193708830000006</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="45">
         <v>6.4323300000000003</v>
       </c>
-      <c r="C36" s="4">
+      <c r="E36" s="45">
         <v>7.6934199999999997</v>
       </c>
-      <c r="D36" s="4">
+      <c r="F36" s="45">
         <v>124.36</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="45">
         <v>6.4300199999999998</v>
       </c>
-      <c r="C37" s="4">
+      <c r="E37" s="45">
         <v>7.6581200000000003</v>
       </c>
-      <c r="D37" s="4">
+      <c r="F37" s="45">
         <v>125.56</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="45">
         <v>6.4204331999999997</v>
       </c>
-      <c r="C38" s="4">
+      <c r="E38" s="45">
         <v>7.8744434999999999</v>
       </c>
-      <c r="D38" s="4">
+      <c r="F38" s="45">
         <v>123.56</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="45">
         <v>6.4203842</v>
       </c>
-      <c r="C39" s="4">
+      <c r="E39" s="45">
         <v>7.0711421999999997</v>
       </c>
-      <c r="D39" s="4">
+      <c r="F39" s="45">
         <v>124.05</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="45">
         <v>6.4099275000000002</v>
       </c>
-      <c r="C40" s="4">
+      <c r="E40" s="45">
         <v>7.9743244999999998</v>
       </c>
-      <c r="D40" s="4">
+      <c r="F40" s="45">
         <v>130.58000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="45">
         <v>6.3635209000000001</v>
       </c>
-      <c r="C41" s="4">
+      <c r="E41" s="45">
         <v>7.9517403</v>
       </c>
-      <c r="D41" s="4">
+      <c r="F41" s="45">
         <v>116.67</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="45">
         <v>6.3406285000000002</v>
       </c>
-      <c r="C42" s="4">
+      <c r="E42" s="45">
         <v>7.7695970000000001</v>
       </c>
-      <c r="D42" s="4">
+      <c r="F42" s="45">
         <v>117.32</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="45">
         <v>6.3379101999999996</v>
       </c>
-      <c r="C43" s="4">
+      <c r="E43" s="45">
         <v>8.0225110999999991</v>
       </c>
-      <c r="D43" s="4">
+      <c r="F43" s="45">
         <v>114.71</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="45">
         <v>6.3241702999999996</v>
       </c>
-      <c r="C44" s="4">
+      <c r="E44" s="45">
         <v>8.1298539000000005</v>
       </c>
-      <c r="D44" s="4">
+      <c r="F44" s="45">
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="45">
         <v>6.3242181000000004</v>
       </c>
-      <c r="C45" s="4">
+      <c r="E45" s="45">
         <v>8.1299449999999993</v>
       </c>
-      <c r="D45" s="4">
+      <c r="F45" s="45">
         <v>74.27</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="45">
         <v>6.3285901999999998</v>
       </c>
-      <c r="C46" s="4">
+      <c r="E46" s="45">
         <v>8.1318555999999997</v>
       </c>
-      <c r="D46" s="4">
+      <c r="F46" s="45">
         <v>63.89</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="45">
         <v>6.3319451000000004</v>
       </c>
-      <c r="C47" s="4">
+      <c r="E47" s="45">
         <v>8.1343788000000004</v>
       </c>
-      <c r="D47" s="4">
+      <c r="F47" s="45">
         <v>60.93</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="45">
         <v>6.3361418</v>
       </c>
-      <c r="C48" s="4">
+      <c r="E48" s="45">
         <v>8.1268809999999991</v>
       </c>
-      <c r="D48" s="4">
+      <c r="F48" s="45">
         <v>75.290000000000006</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="45">
         <v>6.0924312</v>
       </c>
-      <c r="C49" s="4">
+      <c r="E49" s="45">
         <v>6.9174964000000001</v>
       </c>
-      <c r="D49" s="4">
+      <c r="F49" s="45">
         <v>214.34610119999999</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="45">
         <v>6.0923825999999996</v>
       </c>
-      <c r="C50" s="4">
+      <c r="E50" s="45">
         <v>6.9175331</v>
       </c>
-      <c r="D50" s="4">
+      <c r="F50" s="45">
         <v>203.74</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="45">
         <v>6.0926456</v>
       </c>
-      <c r="C51" s="4">
+      <c r="E51" s="45">
         <v>6.9168766000000002</v>
       </c>
-      <c r="D51" s="4">
+      <c r="F51" s="45">
         <v>204.1</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="45">
         <v>6.0919898000000003</v>
       </c>
-      <c r="C52" s="4">
+      <c r="E52" s="45">
         <v>6.9165419000000004</v>
       </c>
-      <c r="D52" s="4">
+      <c r="F52" s="45">
         <v>200.0371026</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="45">
         <v>6.0914336999999996</v>
       </c>
-      <c r="C53" s="4">
+      <c r="E53" s="45">
         <v>6.9178326999999999</v>
       </c>
-      <c r="D53" s="4">
+      <c r="F53" s="45">
         <v>198.74</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="45">
         <v>6.091259</v>
       </c>
-      <c r="C54" s="4">
+      <c r="E54" s="45">
         <v>6.918113</v>
       </c>
-      <c r="D54" s="4">
+      <c r="F54" s="45">
         <v>198.53194260000001</v>
       </c>
     </row>
@@ -1207,169 +1976,236 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" ht="30">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="39">
         <v>7.4342620000000004</v>
       </c>
-      <c r="C2" s="11">
+      <c r="E2" s="39">
         <v>3.9114990000000001</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="39">
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="40">
         <v>7.6167999999999996</v>
       </c>
-      <c r="C3" s="12">
+      <c r="E3" s="40">
         <v>5.2233099999999997</v>
       </c>
-      <c r="D3" s="2">
+      <c r="F3" s="40">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="40">
         <v>7.6215107</v>
       </c>
-      <c r="C4" s="12">
+      <c r="E4" s="40">
         <v>5.221946</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="40">
         <v>438</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="40">
         <v>7.7577509999999998</v>
       </c>
-      <c r="C5" s="12">
+      <c r="E5" s="40">
         <v>5.7218502000000004</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="40">
         <v>539</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
         <v>7.2597199999999997</v>
       </c>
-      <c r="C6" s="11">
+      <c r="E6">
         <v>5.3735080000000002</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="40">
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="39">
         <v>5.2001759999999999</v>
       </c>
-      <c r="C7" s="11">
+      <c r="E7" s="39">
         <v>7.977379</v>
       </c>
-      <c r="D7" s="2">
+      <c r="F7" s="40">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="40">
         <v>5.0272199999999998</v>
       </c>
-      <c r="C8" s="12">
+      <c r="E8" s="40">
         <v>7.9772100000000004</v>
       </c>
-      <c r="D8" s="2">
+      <c r="F8" s="40">
         <v>6</v>
       </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="39">
         <v>6.4075300000000004</v>
       </c>
-      <c r="C9" s="11">
+      <c r="E9" s="39">
         <v>8.2260833000000009</v>
       </c>
-      <c r="D9" s="2">
+      <c r="F9" s="40">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="39">
         <v>6.3096245</v>
       </c>
-      <c r="C10" s="11">
+      <c r="E10" s="39">
         <v>8.1238457999999998</v>
       </c>
-      <c r="D10" s="2">
+      <c r="F10" s="40">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="39">
         <v>6.1087606000000001</v>
       </c>
-      <c r="C11" s="11">
+      <c r="E11" s="39">
         <v>6.9205281999999997</v>
       </c>
-      <c r="D11" s="2">
+      <c r="F11" s="40">
         <v>161</v>
       </c>
     </row>
@@ -1380,1062 +2216,1515 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="5" width="10.5703125" style="1"/>
+    <col min="6" max="6" width="12.85546875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" ht="30" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="9">
         <v>7.5082592999999997</v>
       </c>
-      <c r="C2" s="8">
+      <c r="E2" s="9">
         <v>3.9131901999999998</v>
       </c>
-      <c r="D2" s="8">
+      <c r="F2" s="9">
         <v>262.11297999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="9">
         <v>7.4930361999999997</v>
       </c>
-      <c r="C3" s="8">
+      <c r="E3" s="9">
         <v>3.9171141</v>
       </c>
-      <c r="D3" s="8">
+      <c r="F3" s="9">
         <v>222.8452494</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="9">
         <v>7.4973277999999999</v>
       </c>
-      <c r="C4" s="8">
+      <c r="E4" s="9">
         <v>3.9137483</v>
       </c>
-      <c r="D4" s="8">
+      <c r="F4" s="9">
         <v>254.18005959999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="9">
         <v>7.2126675999999996</v>
       </c>
-      <c r="C5" s="8">
+      <c r="E5" s="9">
         <v>3.8560881999999999</v>
       </c>
-      <c r="D5" s="8">
+      <c r="F5" s="9">
         <v>137.0534126</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="9">
         <v>8.1469462999999998</v>
       </c>
-      <c r="C6" s="8">
+      <c r="E6" s="9">
         <v>4.2385128999999999</v>
       </c>
-      <c r="D6" s="8">
+      <c r="F6" s="9">
         <v>350.97296460000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="13">
         <v>8.1460129000000006</v>
       </c>
-      <c r="C7" s="9">
+      <c r="E7" s="13">
         <v>4.2380645000000001</v>
       </c>
-      <c r="D7" s="9">
+      <c r="F7" s="13">
         <v>347.4895191</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="9">
         <v>8.1492085999999997</v>
       </c>
-      <c r="C8" s="8">
+      <c r="E8" s="9">
         <v>4.2394099000000001</v>
       </c>
-      <c r="D8" s="8">
+      <c r="F8" s="9">
         <v>348.40469519999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="9">
         <v>8.1447479999999999</v>
       </c>
-      <c r="C9" s="8">
+      <c r="E9" s="9">
         <v>4.2379898000000003</v>
       </c>
-      <c r="D9" s="8">
+      <c r="F9" s="9">
         <v>351.41592589999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6" ht="45">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="9">
         <v>8.1054720000000007</v>
       </c>
-      <c r="C10" s="8">
+      <c r="E10" s="9">
         <v>4.2349439999999996</v>
       </c>
-      <c r="D10" s="8">
+      <c r="F10" s="9">
         <v>346.33139999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="9">
         <v>7.7577058000000001</v>
       </c>
-      <c r="C11" s="8">
+      <c r="E11" s="9">
         <v>5.7216997999999997</v>
       </c>
-      <c r="D11" s="8">
+      <c r="F11" s="9">
         <v>562.48781320000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="9">
         <v>7.7487288999999997</v>
       </c>
-      <c r="C12" s="8">
+      <c r="E12" s="9">
         <v>5.6428988999999996</v>
       </c>
-      <c r="D12" s="8">
+      <c r="F12" s="9">
         <v>565.17999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="13">
         <v>7.7433556000000001</v>
       </c>
-      <c r="C13" s="9">
+      <c r="E13" s="13">
         <v>5.6392375000000001</v>
       </c>
-      <c r="D13" s="9">
+      <c r="F13" s="13">
         <v>562.62144560000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="9">
         <v>7.7410205000000003</v>
       </c>
-      <c r="C14" s="8">
+      <c r="E14" s="9">
         <v>5.6431851999999996</v>
       </c>
-      <c r="D14" s="8">
+      <c r="F14" s="9">
         <v>552.81183450000003</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="9">
         <v>7.7408146000000002</v>
       </c>
-      <c r="C15" s="8">
+      <c r="E15" s="9">
         <v>5.6435231999999997</v>
       </c>
-      <c r="D15" s="8">
+      <c r="F15" s="9">
         <v>553.31475450000005</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="9">
         <v>7.6322823</v>
       </c>
-      <c r="C16" s="8">
+      <c r="E16" s="9">
         <v>5.4214238999999997</v>
       </c>
-      <c r="D16" s="8">
+      <c r="F16" s="9">
         <v>419.95606720000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="9">
         <v>7.6383270999999997</v>
       </c>
-      <c r="C17" s="8">
+      <c r="E17" s="9">
         <v>5.4228630999999998</v>
       </c>
-      <c r="D17" s="8">
+      <c r="F17" s="9">
         <v>414.038365</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="13">
         <v>7.6363912000000003</v>
       </c>
-      <c r="C18" s="9">
+      <c r="E18" s="13">
         <v>5.4222919000000003</v>
       </c>
-      <c r="D18" s="9">
+      <c r="F18" s="13">
         <v>421.49562250000002</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="9">
         <v>7.2208299</v>
       </c>
-      <c r="C19" s="8">
+      <c r="E19" s="9">
         <v>5.4022946000000003</v>
       </c>
-      <c r="D19" s="8">
+      <c r="F19" s="9">
         <v>335.24253620000002</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="9">
         <v>7.2155867999999996</v>
       </c>
-      <c r="C20" s="8">
+      <c r="E20" s="9">
         <v>5.4057706000000003</v>
       </c>
-      <c r="D20" s="8">
+      <c r="F20" s="9">
         <v>335.26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="13">
         <v>7.2597208000000002</v>
       </c>
-      <c r="C21" s="9">
+      <c r="E21" s="13">
         <v>5.3735081999999998</v>
       </c>
-      <c r="D21" s="9">
+      <c r="F21" s="13">
         <v>349.38920159999998</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="13">
         <v>7.2590374999999998</v>
       </c>
-      <c r="C22" s="9">
+      <c r="E22" s="13">
         <v>5.3744893999999999</v>
       </c>
-      <c r="D22" s="9">
+      <c r="F22" s="13">
         <v>349.38920159999998</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="13">
         <v>7.2598403999999999</v>
       </c>
-      <c r="C23" s="9">
+      <c r="E23" s="13">
         <v>5.4763064999999997</v>
       </c>
-      <c r="D23" s="9">
+      <c r="F23" s="13">
         <v>323.38337999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="9">
         <v>7.2598403999999999</v>
       </c>
-      <c r="C24" s="8">
+      <c r="E24" s="9">
         <v>5.4763064999999997</v>
       </c>
-      <c r="D24" s="8">
+      <c r="F24" s="9">
         <v>323.38337999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="9">
         <v>8.4588055000000004</v>
       </c>
-      <c r="C25" s="8">
+      <c r="E25" s="9">
         <v>4.5871690000000003</v>
       </c>
-      <c r="D25" s="8">
+      <c r="F25" s="9">
         <v>337.45238499999999</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="9">
         <v>8.4586360999999997</v>
       </c>
-      <c r="C26" s="8">
+      <c r="E26" s="9">
         <v>4.5855233000000002</v>
       </c>
-      <c r="D26" s="8">
+      <c r="F26" s="9">
         <v>332.19378169999999</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="9">
         <v>8.4582362999999994</v>
       </c>
-      <c r="C27" s="8">
+      <c r="E27" s="9">
         <v>4.5883664</v>
       </c>
-      <c r="D27" s="8">
+      <c r="F27" s="9">
         <v>333.20462409999999</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="9">
         <v>8.4580994</v>
       </c>
-      <c r="C28" s="8">
+      <c r="E28" s="9">
         <v>4.5897059000000002</v>
       </c>
-      <c r="D28" s="8">
+      <c r="F28" s="9">
         <v>306.33999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="13">
         <v>8.3884945000000002</v>
       </c>
-      <c r="C29" s="9">
+      <c r="E29" s="13">
         <v>4.5846856999999996</v>
       </c>
-      <c r="D29" s="9">
+      <c r="F29" s="13">
         <v>353.56029910000001</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="9">
         <v>5.0544343999999999</v>
       </c>
-      <c r="C30" s="8">
+      <c r="E30" s="9">
         <v>7.9043095000000001</v>
       </c>
-      <c r="D30" s="8">
+      <c r="F30" s="9">
         <v>78.057799200000005</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="9">
         <v>5.0571232000000004</v>
       </c>
-      <c r="C31" s="8">
+      <c r="E31" s="9">
         <v>7.9037034999999998</v>
       </c>
-      <c r="D31" s="8">
+      <c r="F31" s="9">
         <v>92.203197009999997</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="9">
         <v>5.0560362999999997</v>
       </c>
-      <c r="C32" s="8">
+      <c r="E32" s="9">
         <v>7.9007921999999997</v>
       </c>
-      <c r="D32" s="8">
+      <c r="F32" s="9">
         <v>87.837404199999995</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="9">
         <v>5.0577817999999999</v>
       </c>
-      <c r="C33" s="8">
+      <c r="E33" s="9">
         <v>7.9020660999999999</v>
       </c>
-      <c r="D33" s="8">
+      <c r="F33" s="9">
         <v>90.913150470000005</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="9">
         <v>5.0546939000000002</v>
       </c>
-      <c r="C34" s="8">
+      <c r="E34" s="9">
         <v>7.9160988000000003</v>
       </c>
-      <c r="D34" s="8">
+      <c r="F34" s="9">
         <v>93.96233909</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:6" ht="45">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="9">
         <v>5.0434536000000003</v>
       </c>
-      <c r="C35" s="8">
+      <c r="E35" s="9">
         <v>7.8791330000000004</v>
       </c>
-      <c r="D35" s="8">
+      <c r="F35" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:6" ht="45">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="13">
         <v>5.0394893999999999</v>
       </c>
-      <c r="C36" s="9">
+      <c r="E36" s="13">
         <v>7.8731235000000002</v>
       </c>
-      <c r="D36" s="9">
+      <c r="F36" s="13">
         <v>79.298878619999996</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:6" ht="45">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="9">
         <v>5.0400241000000001</v>
       </c>
-      <c r="C37" s="8">
+      <c r="E37" s="9">
         <v>7.8734451999999999</v>
       </c>
-      <c r="D37" s="8">
+      <c r="F37" s="9">
         <v>81.819504260000002</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:6" ht="45">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="9">
         <v>5.0406405999999997</v>
       </c>
-      <c r="C38" s="8">
+      <c r="E38" s="9">
         <v>7.8738900000000003</v>
       </c>
-      <c r="D38" s="8">
+      <c r="F38" s="9">
         <v>85.720904570000002</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:6" ht="45">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="9">
         <v>5.0409587</v>
       </c>
-      <c r="C39" s="8">
+      <c r="E39" s="9">
         <v>7.8737336999999998</v>
       </c>
-      <c r="D39" s="8">
+      <c r="F39" s="9">
         <v>84.218533309999998</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="9">
         <v>5.0410715000000001</v>
       </c>
-      <c r="C40" s="8">
+      <c r="E40" s="9">
         <v>7.8727042999999997</v>
       </c>
-      <c r="D40" s="8">
+      <c r="F40" s="9">
         <v>82.90707639</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="9">
         <v>5.0411717999999999</v>
       </c>
-      <c r="C41" s="8">
+      <c r="E41" s="9">
         <v>7.8724673000000003</v>
       </c>
-      <c r="D41" s="8">
+      <c r="F41" s="9">
         <v>79.798794009999995</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="9">
         <v>5.0422811000000003</v>
       </c>
-      <c r="C42" s="8">
+      <c r="E42" s="9">
         <v>7.8696457000000004</v>
       </c>
-      <c r="D42" s="8">
+      <c r="F42" s="9">
         <v>72.167455590000003</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="9">
         <v>5.0422913999999999</v>
       </c>
-      <c r="C43" s="8">
+      <c r="E43" s="9">
         <v>7.8696792000000002</v>
       </c>
-      <c r="D43" s="8">
+      <c r="F43" s="9">
         <v>78.193708830000006</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="9">
         <v>6.4323300000000003</v>
       </c>
-      <c r="C44" s="8">
+      <c r="E44" s="9">
         <v>7.6934199999999997</v>
       </c>
-      <c r="D44" s="8">
+      <c r="F44" s="9">
         <v>124.36</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="9">
         <v>6.4300199999999998</v>
       </c>
-      <c r="C45" s="8">
+      <c r="E45" s="9">
         <v>7.6581200000000003</v>
       </c>
-      <c r="D45" s="8">
+      <c r="F45" s="9">
         <v>125.56</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="9">
         <v>6.4911640000000004</v>
       </c>
-      <c r="C46" s="8">
+      <c r="E46" s="9">
         <v>7.7033399999999999</v>
       </c>
-      <c r="D46" s="8">
+      <c r="F46" s="9">
         <v>124.95</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:6" ht="60">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="9">
         <v>6.4204331999999997</v>
       </c>
-      <c r="C47" s="8">
+      <c r="E47" s="9">
         <v>7.8744434999999999</v>
       </c>
-      <c r="D47" s="8">
+      <c r="F47" s="9">
         <v>123.56</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="9">
         <v>6.4203842</v>
       </c>
-      <c r="C48" s="8">
+      <c r="E48" s="9">
         <v>7.0711421999999997</v>
       </c>
-      <c r="D48" s="8">
+      <c r="F48" s="9">
         <v>124.05</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:6" ht="45">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="9">
         <v>6.4099275000000002</v>
       </c>
-      <c r="C49" s="8">
+      <c r="E49" s="9">
         <v>7.9743244999999998</v>
       </c>
-      <c r="D49" s="8">
+      <c r="F49" s="9">
         <v>130.58000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="9">
         <v>6.3635209000000001</v>
       </c>
-      <c r="C50" s="8">
+      <c r="E50" s="9">
         <v>7.9517403</v>
       </c>
-      <c r="D50" s="8">
+      <c r="F50" s="9">
         <v>116.67</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="9">
         <v>6.3406285000000002</v>
       </c>
-      <c r="C51" s="8">
+      <c r="E51" s="9">
         <v>7.7695970000000001</v>
       </c>
-      <c r="D51" s="8">
+      <c r="F51" s="9">
         <v>117.32</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:6" ht="45">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="9">
         <v>6.3379101999999996</v>
       </c>
-      <c r="C52" s="8">
+      <c r="E52" s="9">
         <v>8.0225110999999991</v>
       </c>
-      <c r="D52" s="8">
+      <c r="F52" s="9">
         <v>114.71</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:6" ht="45">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="9">
         <v>6.3293100000000004</v>
       </c>
-      <c r="C53" s="8">
+      <c r="E53" s="9">
         <v>7.9810999999999996</v>
       </c>
-      <c r="D53" s="8">
+      <c r="F53" s="9">
         <v>115.05</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:6" ht="30">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="9">
         <v>6.3241702999999996</v>
       </c>
-      <c r="C54" s="8">
+      <c r="E54" s="9">
         <v>8.1298539000000005</v>
       </c>
-      <c r="D54" s="8">
+      <c r="F54" s="9">
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:6" ht="30">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="9">
         <v>6.3242181000000004</v>
       </c>
-      <c r="C55" s="8">
+      <c r="E55" s="9">
         <v>8.1299449999999993</v>
       </c>
-      <c r="D55" s="8">
+      <c r="F55" s="9">
         <v>74.27</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="9">
         <v>6.3285901999999998</v>
       </c>
-      <c r="C56" s="8">
+      <c r="E56" s="9">
         <v>8.1318555999999997</v>
       </c>
-      <c r="D56" s="8">
+      <c r="F56" s="9">
         <v>63.89</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="9">
         <v>6.3319451000000004</v>
       </c>
-      <c r="C57" s="8">
+      <c r="E57" s="9">
         <v>8.1343788000000004</v>
       </c>
-      <c r="D57" s="8">
+      <c r="F57" s="9">
         <v>60.93</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:6" ht="45">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D58" s="9">
         <v>6.3361418</v>
       </c>
-      <c r="C58" s="8">
+      <c r="E58" s="9">
         <v>8.1268809999999991</v>
       </c>
-      <c r="D58" s="8">
+      <c r="F58" s="9">
         <v>75.290000000000006</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="9">
         <v>6.0924312</v>
       </c>
-      <c r="C59" s="8">
+      <c r="E59" s="9">
         <v>6.9174964000000001</v>
       </c>
-      <c r="D59" s="8">
+      <c r="F59" s="9">
         <v>214.34610119999999</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" s="9">
         <v>6.0923825999999996</v>
       </c>
-      <c r="C60" s="8">
+      <c r="E60" s="9">
         <v>6.9175331</v>
       </c>
-      <c r="D60" s="8">
+      <c r="F60" s="9">
         <v>203.74</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" s="9">
         <v>6.0926456</v>
       </c>
-      <c r="C61" s="8">
+      <c r="E61" s="9">
         <v>6.9168766000000002</v>
       </c>
-      <c r="D61" s="8">
+      <c r="F61" s="9">
         <v>204.1</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D62" s="9">
         <v>6.0919898000000003</v>
       </c>
-      <c r="C62" s="8">
+      <c r="E62" s="9">
         <v>6.9165419000000004</v>
       </c>
-      <c r="D62" s="8">
+      <c r="F62" s="9">
         <v>200.0371026</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B63" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="9">
         <v>6.0914336999999996</v>
       </c>
-      <c r="C63" s="8">
+      <c r="E63" s="9">
         <v>6.9178326999999999</v>
       </c>
-      <c r="D63" s="8">
+      <c r="F63" s="9">
         <v>198.74</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" s="9">
         <v>6.091259</v>
       </c>
-      <c r="C64" s="8">
+      <c r="E64" s="9">
         <v>6.918113</v>
       </c>
-      <c r="D64" s="8">
+      <c r="F64" s="9">
         <v>198.53194260000001</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D65" s="9">
         <v>6.0976999999999997</v>
       </c>
-      <c r="C65" s="8">
+      <c r="E65" s="9">
         <v>6.9177</v>
       </c>
-      <c r="D65" s="8">
+      <c r="F65" s="9">
         <v>204.09</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="35">
         <v>7.4342620000000004</v>
       </c>
-      <c r="C66" s="1">
+      <c r="E66" s="35">
         <v>3.9114990000000001</v>
       </c>
-      <c r="D66" s="1">
+      <c r="F66" s="35">
         <v>227</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="36">
         <v>7.6167999999999996</v>
       </c>
-      <c r="C67" s="2">
+      <c r="E67" s="36">
         <v>5.2233099999999997</v>
       </c>
-      <c r="D67" s="2">
+      <c r="F67" s="36">
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="36">
         <v>7.6215107</v>
       </c>
-      <c r="C68" s="2">
+      <c r="E68" s="36">
         <v>5.221946</v>
       </c>
-      <c r="D68" s="2">
+      <c r="F68" s="36">
         <v>438</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="36">
         <v>7.7577509999999998</v>
       </c>
-      <c r="C69" s="2">
+      <c r="E69" s="36">
         <v>5.7218502000000004</v>
       </c>
-      <c r="D69" s="2">
+      <c r="F69" s="36">
         <v>539</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" s="1">
         <v>7.2597199999999997</v>
       </c>
-      <c r="C70">
+      <c r="E70" s="1">
         <v>5.3735080000000002</v>
       </c>
-      <c r="D70" s="2">
+      <c r="F70" s="36">
         <v>349</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" s="35">
         <v>5.2001759999999999</v>
       </c>
-      <c r="C71" s="1">
+      <c r="E71" s="35">
         <v>7.977379</v>
       </c>
-      <c r="D71" s="2">
+      <c r="F71" s="36">
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" s="36">
         <v>5.0272199999999998</v>
       </c>
-      <c r="C72" s="2">
+      <c r="E72" s="36">
         <v>7.9772100000000004</v>
       </c>
-      <c r="D72" s="2">
+      <c r="F72" s="36">
         <v>6</v>
       </c>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5">
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" s="35">
         <v>6.4075300000000004</v>
       </c>
-      <c r="C73" s="1">
+      <c r="E73" s="35">
         <v>8.2260833000000009</v>
       </c>
-      <c r="D73" s="2">
+      <c r="F73" s="36">
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="35">
         <v>6.3096245</v>
       </c>
-      <c r="C74" s="1">
+      <c r="E74" s="35">
         <v>8.1238457999999998</v>
       </c>
-      <c r="D74" s="2">
+      <c r="F74" s="36">
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" s="35">
         <v>6.1087606000000001</v>
       </c>
-      <c r="C75" s="1">
+      <c r="E75" s="35">
         <v>6.9205281999999997</v>
       </c>
-      <c r="D75" s="2">
+      <c r="F75" s="36">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added my updated plot
</commit_message>
<xml_diff>
--- a/Data/maps.xlsx
+++ b/Data/maps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Farms" sheetId="4" r:id="rId1"/>
@@ -220,6 +220,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -233,6 +234,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -241,6 +243,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>unhufu</t>
     </r>
@@ -265,7 +268,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -273,30 +276,32 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -304,7 +309,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -430,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -479,11 +484,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -600,6 +616,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -879,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1659,13 +1678,13 @@
       <c r="C39" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="45">
+      <c r="D39" s="9">
         <v>6.4203842</v>
       </c>
-      <c r="E39" s="45">
-        <v>7.0711421999999997</v>
-      </c>
-      <c r="F39" s="45">
+      <c r="E39" s="46">
+        <v>7.8733303000000001</v>
+      </c>
+      <c r="F39" s="9">
         <v>124.05</v>
       </c>
     </row>
@@ -2218,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3181,8 +3200,8 @@
       <c r="D48" s="9">
         <v>6.4203842</v>
       </c>
-      <c r="E48" s="9">
-        <v>7.0711421999999997</v>
+      <c r="E48" s="46">
+        <v>7.8733303000000001</v>
       </c>
       <c r="F48" s="9">
         <v>124.05</v>

</xml_diff>